<commit_message>
update test case register page
update register page
</commit_message>
<xml_diff>
--- a/Documents/FM_test case register page.xlsx
+++ b/Documents/FM_test case register page.xlsx
@@ -63,9 +63,6 @@
     <t>Check giao diện</t>
   </si>
   <si>
-    <t>trang register</t>
-  </si>
-  <si>
     <t>điền thông tin đăng nhập</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>hiện thông báo "đăng ký không thành công " , thông báo chỗ sai</t>
+  </si>
+  <si>
+    <t>trang Register</t>
   </si>
 </sst>
 </file>
@@ -228,22 +228,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -253,6 +241,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,7 +558,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -636,14 +636,14 @@
         <f>A8+1</f>
         <v>2</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
@@ -658,15 +658,15 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" ref="A10:A18" si="0">A9+1</f>
-        <v>3</v>
-      </c>
-      <c r="B10" s="11"/>
+        <f t="shared" ref="A10:A16" si="0">A9+1</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="18"/>
       <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -684,12 +684,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
@@ -707,12 +707,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6">
@@ -730,12 +730,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
@@ -753,12 +753,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
@@ -777,13 +777,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
@@ -801,12 +801,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
@@ -820,24 +820,24 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>